<commit_message>
Update to api list
</commit_message>
<xml_diff>
--- a/04_API/Danam_API_List.xlsx
+++ b/04_API/Danam_API_List.xlsx
@@ -310,10 +310,10 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -322,28 +322,28 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -368,8 +368,8 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffb0eb9a"/>
       <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffb0eb9a"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1471,13 +1471,13 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="10">
+      <c r="A6" t="s" s="16">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="11">
+      <c r="B6" t="s" s="17">
         <v>2</v>
       </c>
-      <c r="C6" t="s" s="12">
+      <c r="C6" t="s" s="18">
         <v>6</v>
       </c>
       <c r="D6" s="13"/>
@@ -1486,13 +1486,13 @@
       <c r="G6" s="13"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="10">
+      <c r="A7" t="s" s="16">
         <v>7</v>
       </c>
-      <c r="B7" t="s" s="11">
+      <c r="B7" t="s" s="17">
         <v>2</v>
       </c>
-      <c r="C7" t="s" s="12">
+      <c r="C7" t="s" s="18">
         <v>6</v>
       </c>
       <c r="D7" s="13"/>
@@ -1501,13 +1501,13 @@
       <c r="G7" s="13"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="10">
+      <c r="A8" t="s" s="16">
         <v>8</v>
       </c>
-      <c r="B8" t="s" s="11">
+      <c r="B8" t="s" s="17">
         <v>2</v>
       </c>
-      <c r="C8" t="s" s="12">
+      <c r="C8" t="s" s="18">
         <v>3</v>
       </c>
       <c r="D8" s="13"/>
@@ -1516,13 +1516,13 @@
       <c r="G8" s="13"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="10">
+      <c r="A9" t="s" s="16">
         <v>9</v>
       </c>
-      <c r="B9" t="s" s="11">
+      <c r="B9" t="s" s="17">
         <v>2</v>
       </c>
-      <c r="C9" t="s" s="12">
+      <c r="C9" t="s" s="18">
         <v>3</v>
       </c>
       <c r="D9" s="13"/>
@@ -1540,13 +1540,13 @@
       <c r="G10" s="13"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="16">
+      <c r="A11" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="17">
+      <c r="B11" t="s" s="11">
         <v>11</v>
       </c>
-      <c r="C11" t="s" s="18">
+      <c r="C11" t="s" s="12">
         <v>6</v>
       </c>
       <c r="D11" s="13"/>
@@ -1555,13 +1555,13 @@
       <c r="G11" s="13"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="16">
+      <c r="A12" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="B12" t="s" s="17">
+      <c r="B12" t="s" s="11">
         <v>11</v>
       </c>
-      <c r="C12" t="s" s="18">
+      <c r="C12" t="s" s="12">
         <v>6</v>
       </c>
       <c r="D12" s="13"/>
@@ -1579,13 +1579,13 @@
       <c r="G13" s="13"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="10">
+      <c r="A14" t="s" s="16">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="11">
+      <c r="B14" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="C14" t="s" s="12">
+      <c r="C14" t="s" s="18">
         <v>3</v>
       </c>
       <c r="D14" s="13"/>
@@ -1594,13 +1594,13 @@
       <c r="G14" s="13"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="16">
+      <c r="A15" t="s" s="10">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="17">
+      <c r="B15" t="s" s="11">
         <v>2</v>
       </c>
-      <c r="C15" t="s" s="18">
+      <c r="C15" t="s" s="12">
         <v>6</v>
       </c>
       <c r="D15" s="13"/>
@@ -1618,13 +1618,13 @@
       <c r="G16" s="13"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="10">
+      <c r="A17" t="s" s="16">
         <v>15</v>
       </c>
-      <c r="B17" t="s" s="11">
+      <c r="B17" t="s" s="17">
         <v>2</v>
       </c>
-      <c r="C17" t="s" s="12">
+      <c r="C17" t="s" s="18">
         <v>3</v>
       </c>
       <c r="D17" s="13"/>
@@ -1642,13 +1642,13 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="16">
+      <c r="A19" t="s" s="10">
         <v>16</v>
       </c>
-      <c r="B19" t="s" s="17">
+      <c r="B19" t="s" s="11">
         <v>11</v>
       </c>
-      <c r="C19" t="s" s="18">
+      <c r="C19" t="s" s="12">
         <v>6</v>
       </c>
       <c r="D19" s="13"/>
@@ -1666,7 +1666,7 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="10">
+      <c r="A21" t="s" s="16">
         <v>17</v>
       </c>
       <c r="B21" s="15"/>
@@ -1677,7 +1677,7 @@
       <c r="G21" s="13"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="10">
+      <c r="A22" t="s" s="16">
         <v>18</v>
       </c>
       <c r="B22" s="15"/>

</xml_diff>